<commit_message>
edicion de matrices de coexistencia en R que genero varios archivos .csv y .txt en la carpeta Data/coexistence_Analysis. Creacion de matriz con los datos de las dos localidades para analisis de coexistencia. Los analisisy arreglo de datos estan hechos en el script coexistencia.R. Ademas cree el excel Result_Coexistence para sumarizar los resultados
</commit_message>
<xml_diff>
--- a/Data/Coexistence_Analysis/Matrices_por_estrato.xlsx
+++ b/Data/Coexistence_Analysis/Matrices_por_estrato.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MS_in_prep\Orquis\Data\Community_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MS_in_prep\Orquis\Data\Coexistence_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="LH_E1" sheetId="1" r:id="rId1"/>
@@ -39,105 +39,6 @@
   </si>
   <si>
     <t>stratum</t>
-  </si>
-  <si>
-    <t>Campylocentrum.micranthum</t>
-  </si>
-  <si>
-    <t>Cryptocentrum.latifolium</t>
-  </si>
-  <si>
-    <t>Dichaea.hystricina</t>
-  </si>
-  <si>
-    <t>Dichaea.pendula</t>
-  </si>
-  <si>
-    <t>Encyclia.prostechea</t>
-  </si>
-  <si>
-    <t>Epidendrum.LH</t>
-  </si>
-  <si>
-    <t>Epidendrum.porpax</t>
-  </si>
-  <si>
-    <t>Epidendrum.RY</t>
-  </si>
-  <si>
-    <t>Epidendrum.sp.1</t>
-  </si>
-  <si>
-    <t>Lankesteriana.cuspidata</t>
-  </si>
-  <si>
-    <t>Lepanthes.sp</t>
-  </si>
-  <si>
-    <t>Lepanthes.sp.1</t>
-  </si>
-  <si>
-    <t>Lepanthes.sp.2</t>
-  </si>
-  <si>
-    <t>Lepanthes.sp.3</t>
-  </si>
-  <si>
-    <t>Lepanthopsis.floripecten</t>
-  </si>
-  <si>
-    <t>Maxillaria</t>
-  </si>
-  <si>
-    <t>Maxillaria.fritzii</t>
-  </si>
-  <si>
-    <t>Maxillaria.ochracea</t>
-  </si>
-  <si>
-    <t>Mormolyca.rufescens</t>
-  </si>
-  <si>
-    <t>Myoxanthus.affinis</t>
-  </si>
-  <si>
-    <t>Oncidium.adelaide</t>
-  </si>
-  <si>
-    <t>Oncidium.chrysomorphum</t>
-  </si>
-  <si>
-    <t>Oncidium.pictum</t>
-  </si>
-  <si>
-    <t>Platystele.consobrina</t>
-  </si>
-  <si>
-    <t>Pleurothallis.hystrix</t>
-  </si>
-  <si>
-    <t>Pleurothallis.tripterantha</t>
-  </si>
-  <si>
-    <t>Restrepia.antennifera</t>
-  </si>
-  <si>
-    <t>Stelis.argentata</t>
-  </si>
-  <si>
-    <t>Stelis.popayanensis</t>
-  </si>
-  <si>
-    <t>Stelis.sp.1</t>
-  </si>
-  <si>
-    <t>Stelis.sp.2</t>
-  </si>
-  <si>
-    <t>Stelis.spathulata</t>
-  </si>
-  <si>
-    <t>Stelis.vulcanica</t>
   </si>
   <si>
     <t>F01</t>
@@ -218,7 +119,106 @@
     <t>RY</t>
   </si>
   <si>
-    <t>Sigmatostalix.sergii</t>
+    <t>C_mic</t>
+  </si>
+  <si>
+    <t>C_lat</t>
+  </si>
+  <si>
+    <t>D_hys</t>
+  </si>
+  <si>
+    <t>D_pen</t>
+  </si>
+  <si>
+    <t>E_pro</t>
+  </si>
+  <si>
+    <t>Epi_lh</t>
+  </si>
+  <si>
+    <t>E_por</t>
+  </si>
+  <si>
+    <t>Epi_ry</t>
+  </si>
+  <si>
+    <t>Epi_1</t>
+  </si>
+  <si>
+    <t>L_cus</t>
+  </si>
+  <si>
+    <t>Lep_sp</t>
+  </si>
+  <si>
+    <t>Lep_sp1</t>
+  </si>
+  <si>
+    <t>Lep_sp2</t>
+  </si>
+  <si>
+    <t>Lep_sp3</t>
+  </si>
+  <si>
+    <t>L_flo</t>
+  </si>
+  <si>
+    <t>Max_sp</t>
+  </si>
+  <si>
+    <t>M_fri</t>
+  </si>
+  <si>
+    <t>M_och</t>
+  </si>
+  <si>
+    <t>M_ruf</t>
+  </si>
+  <si>
+    <t>M_aff</t>
+  </si>
+  <si>
+    <t>O_ade</t>
+  </si>
+  <si>
+    <t>O_chr</t>
+  </si>
+  <si>
+    <t>O_pic</t>
+  </si>
+  <si>
+    <t>P_con</t>
+  </si>
+  <si>
+    <t>P_hys</t>
+  </si>
+  <si>
+    <t>P_tri</t>
+  </si>
+  <si>
+    <t>R_ant</t>
+  </si>
+  <si>
+    <t>S_arg</t>
+  </si>
+  <si>
+    <t>S_pop</t>
+  </si>
+  <si>
+    <t>Ste_sp1</t>
+  </si>
+  <si>
+    <t>Ste_sp2</t>
+  </si>
+  <si>
+    <t>S_spa</t>
+  </si>
+  <si>
+    <t>S_vul</t>
+  </si>
+  <si>
+    <t>S_ser</t>
   </si>
 </sst>
 </file>
@@ -538,118 +538,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection sqref="A1:AK10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -657,13 +659,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -770,13 +772,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -883,13 +885,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -996,13 +998,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1109,13 +1111,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1222,13 +1224,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1335,13 +1337,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1448,13 +1450,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1561,13 +1563,13 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1685,120 +1687,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -1806,13 +1808,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1919,13 +1921,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2032,13 +2034,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2145,13 +2147,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2258,13 +2260,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2371,13 +2373,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2484,13 +2486,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2597,13 +2599,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2717,120 +2719,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:AK79"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -2838,13 +2840,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2951,13 +2953,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3064,13 +3066,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3177,13 +3179,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3290,13 +3292,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3403,13 +3405,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3516,13 +3518,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3629,13 +3631,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3749,120 +3751,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:AK71"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -3870,13 +3872,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3983,13 +3985,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -4096,13 +4098,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4209,13 +4211,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -4322,13 +4324,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -4435,13 +4437,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4548,13 +4550,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -4661,13 +4663,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -4774,13 +4776,13 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -4894,120 +4896,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:AK62"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -5015,13 +5017,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5128,13 +5130,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -5241,13 +5243,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -5354,13 +5356,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5467,13 +5469,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -5580,13 +5582,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -5693,13 +5695,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -5806,13 +5808,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -5919,13 +5921,13 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -6039,120 +6041,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:AK53"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -6160,13 +6162,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6273,13 +6275,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -6386,13 +6388,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -6499,13 +6501,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -6612,13 +6614,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6725,13 +6727,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -6838,13 +6840,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6951,13 +6953,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -7071,120 +7073,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:AK45"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -7192,13 +7194,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -7305,13 +7307,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -7418,13 +7420,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -7531,13 +7533,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -7644,13 +7646,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -7757,13 +7759,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -7870,13 +7872,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7983,13 +7985,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -8096,13 +8098,13 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -8216,120 +8218,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:AK36"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -8337,13 +8339,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -8450,13 +8452,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -8563,13 +8565,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -8676,13 +8678,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -8789,13 +8791,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -8902,13 +8904,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -9015,13 +9017,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -9128,13 +9130,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -9241,13 +9243,13 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -9361,120 +9363,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:AK27"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -9482,13 +9484,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9595,13 +9597,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -9708,13 +9710,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -9821,13 +9823,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -9934,13 +9936,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -10047,13 +10049,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -10160,13 +10162,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -10273,13 +10275,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -10386,13 +10388,13 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -10506,120 +10508,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:AK18"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AK1" t="s">
         <v>61</v>
@@ -10627,13 +10629,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -10740,13 +10742,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -10853,13 +10855,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -10966,13 +10968,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -11079,13 +11081,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -11192,13 +11194,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -11305,13 +11307,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -11418,13 +11420,13 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -11531,13 +11533,13 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>1</v>

</xml_diff>

<commit_message>
en orquis_MS agregue el plan de analisis para corroborar el titulo del abstract del sibecol. El cambio en matrices por estato.xls es superficial y no afecta a los datos preexistentes.
</commit_message>
<xml_diff>
--- a/Data/Coexistence_Analysis/Matrices_por_estrato.xlsx
+++ b/Data/Coexistence_Analysis/Matrices_por_estrato.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LH_E1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="66">
   <si>
     <t>tree</t>
   </si>
@@ -220,6 +220,18 @@
   <si>
     <t>S_ser</t>
   </si>
+  <si>
+    <t>Bloque Lepanthes, Lepanthopsis, Campylocentrum.</t>
+  </si>
+  <si>
+    <t>Bloque de Stelis spathulata, Restrepia y Oncidium pictum.</t>
+  </si>
+  <si>
+    <t>Bloque R. ant, S. spa, O. pic</t>
+  </si>
+  <si>
+    <t>Bloque Lepanthes, C. mic</t>
+  </si>
 </sst>
 </file>
 
@@ -234,12 +246,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,8 +284,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1687,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:AK9"/>
     </sheetView>
   </sheetViews>
@@ -4894,15 +4927,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK10"/>
+  <dimension ref="A1:BC13"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AK10"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AO18" sqref="AO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -5014,8 +5047,59 @@
       <c r="AK1" t="s">
         <v>61</v>
       </c>
+      <c r="AM1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -5127,8 +5211,59 @@
       <c r="AK2">
         <v>0</v>
       </c>
+      <c r="AM2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -5240,8 +5375,59 @@
       <c r="AK3">
         <v>0</v>
       </c>
+      <c r="AM3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -5353,8 +5539,59 @@
       <c r="AK4">
         <v>0</v>
       </c>
+      <c r="AM4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>1</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -5466,8 +5703,59 @@
       <c r="AK5">
         <v>0</v>
       </c>
+      <c r="AM5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -5579,8 +5867,59 @@
       <c r="AK6">
         <v>0</v>
       </c>
+      <c r="AM6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>1</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>1</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>1</v>
+      </c>
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -5692,8 +6031,59 @@
       <c r="AK7">
         <v>0</v>
       </c>
+      <c r="AM7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -5805,8 +6195,59 @@
       <c r="AK8">
         <v>0</v>
       </c>
+      <c r="AM8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>1</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5918,8 +6359,59 @@
       <c r="AK9">
         <v>0</v>
       </c>
+      <c r="AM9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>1</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA9" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -6030,6 +6522,67 @@
       </c>
       <c r="AK10">
         <v>0</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA10" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
+      <c r="BC10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AN12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AN13" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -6039,15 +6592,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK9"/>
+  <dimension ref="A1:BB13"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AK9"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AO15" sqref="AO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -6159,8 +6712,56 @@
       <c r="AK1" t="s">
         <v>61</v>
       </c>
+      <c r="AM1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -6272,8 +6873,56 @@
       <c r="AK2">
         <v>0</v>
       </c>
+      <c r="AM2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -6385,8 +7034,56 @@
       <c r="AK3">
         <v>0</v>
       </c>
+      <c r="AM3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -6498,8 +7195,56 @@
       <c r="AK4">
         <v>0</v>
       </c>
+      <c r="AM4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>1</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -6611,8 +7356,56 @@
       <c r="AK5">
         <v>0</v>
       </c>
+      <c r="AM5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>1</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>1</v>
+      </c>
+      <c r="BA5">
+        <v>1</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -6724,8 +7517,56 @@
       <c r="AK6">
         <v>0</v>
       </c>
+      <c r="AM6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+      <c r="AR6">
+        <v>1</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA6">
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -6837,8 +7678,56 @@
       <c r="AK7">
         <v>0</v>
       </c>
+      <c r="AM7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ7" s="3">
+        <v>1</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6950,8 +7839,56 @@
       <c r="AK8">
         <v>0</v>
       </c>
+      <c r="AM8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>1</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ8" s="3">
+        <v>1</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -7062,6 +7999,64 @@
       </c>
       <c r="AK9">
         <v>1</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>1</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ9" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AO12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AO13" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>